<commit_message>
Add Roadmap_Milestone dropdown validation
</commit_message>
<xml_diff>
--- a/data/Project_Aion_PM_System.xlsx
+++ b/data/Project_Aion_PM_System.xlsx
@@ -12,6 +12,7 @@
     <sheet name="04_Tickets" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="05_Dashboard" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="06_Decisions_Log" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="99_Validation" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1095,6 +1096,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="15" t="inlineStr">
         <is>
@@ -2720,6 +2722,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="15" t="inlineStr">
         <is>
@@ -3413,7 +3416,7 @@
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation sqref="F5:F200" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"P0,P1,P2,P3"</formula1>
     </dataValidation>
@@ -3422,6 +3425,12 @@
     </dataValidation>
     <dataValidation sqref="G5:G200" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Backlog,Not started,In progress,Blocked,Ready for review,Done"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q5:Q19" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>'99_Validation'!$A$2:$A$16</formula1>
+    </dataValidation>
+    <dataValidation sqref="S5:S19" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>'99_Validation'!$B$2:$B$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4139,4 +4148,160 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Allowed_Realms</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Allowed_Roadmap_Milestones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>00_Triage_Inbox</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Q1_2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01_Project_Framework</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Q2_2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Q3_2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03_Artifacts</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Q4_2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04_Admin_Automation_AWACS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05_IT_Infrastructure</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06_Databases</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07_Expert_Systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>08_Modelling_Feature_Design_and_Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>09_ML_AI_Systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10_Model_Simulation_Backtesting</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11_Trading_Strategies</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12_Trading_Engines</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13_Business_Intelligence</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Framework_Directory_Spec__legacy</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Set Project Aion PM System aligned to Framework Index
</commit_message>
<xml_diff>
--- a/data/Project_Aion_PM_System.xlsx
+++ b/data/Project_Aion_PM_System.xlsx
@@ -13,6 +13,10 @@
     <sheet name="05_Dashboard" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="06_Decisions_Log" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="99_Validation" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Framework_Index" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Framework_Coverage" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Review_Roadmap" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Review_Tickets" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -832,7 +836,7 @@
     <row r="4" ht="360" customHeight="1" s="12">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Project vision (1–2 sentences)</t>
+          <t>Project Vision</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
@@ -1056,13 +1060,579 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Row</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suggested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Confidence</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Top3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market (0.10), 37_Trading_Strategies_cA_Continuous_Alpha (0.10), 41_Trading_Strategies_Staking_Kelly (0.09)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market (0.11), 05_Glass_Cockpit_GUI (0.10), 02_Technology_Advantage (0.09)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Row</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Suggested</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Confidence</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Top3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers (0.10), 40_Business_Intelligence_Reconciliation (0.09), 39_Business_Intelligence_Reporting (0.09)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI (0.12), 24_Features_Public_Live_Market (0.10), 11_GUI_Pulse_Input (0.10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -1088,6 +1658,26 @@
           <t>High‑Level Roadmap (Epics)</t>
         </is>
       </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Framework_Suggested</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Framework_Confidence</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Framework_Top3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="inlineStr">
@@ -1095,6 +1685,29 @@
           <t>Baseline created: 2026-01-23  |  Adjust dates/owners freely.</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market (0.10), 37_Trading_Strategies_cA_Continuous_Alpha (0.10), 41_Trading_Strategies_Staking_Kelly (0.09)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="15" t="inlineStr">
@@ -1147,6 +1760,24 @@
           <t>Notes</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market (0.11), 05_Glass_Cockpit_GUI (0.10), 02_Technology_Advantage (0.09)</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="42" customHeight="1" s="12">
       <c r="A5" s="5" t="inlineStr">
@@ -1193,6 +1824,24 @@
           <t>Sets up operating rhythm</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="42" customHeight="1" s="12">
       <c r="A6" s="5" t="inlineStr">
@@ -1239,6 +1888,24 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="42" customHeight="1" s="12">
       <c r="A7" s="5" t="inlineStr">
@@ -1289,6 +1956,24 @@
           <t>POWRTG/SPDRTG/MRKRTG/TRKSPD/Time Standards</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="42" customHeight="1" s="12">
       <c r="A8" s="5" t="inlineStr">
@@ -1335,6 +2020,24 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="42" customHeight="1" s="12">
       <c r="A9" s="5" t="inlineStr">
@@ -1381,6 +2084,24 @@
         </is>
       </c>
       <c r="J9" s="5" t="n"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="42" customHeight="1" s="12">
       <c r="A10" s="5" t="inlineStr">
@@ -1427,6 +2148,24 @@
         </is>
       </c>
       <c r="J10" s="5" t="n"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="42" customHeight="1" s="12">
       <c r="A11" s="5" t="inlineStr">
@@ -1473,6 +2212,24 @@
         </is>
       </c>
       <c r="J11" s="5" t="n"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="42" customHeight="1" s="12">
       <c r="A12" s="5" t="inlineStr">
@@ -1519,6 +2276,24 @@
         </is>
       </c>
       <c r="J12" s="5" t="n"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="42" customHeight="1" s="12">
       <c r="A13" s="5" t="inlineStr">
@@ -1565,6 +2340,24 @@
         </is>
       </c>
       <c r="J13" s="5" t="n"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="42" customHeight="1" s="12">
       <c r="A14" s="5" t="inlineStr">
@@ -1611,6 +2404,24 @@
         </is>
       </c>
       <c r="J14" s="5" t="n"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="42" customHeight="1" s="12">
       <c r="A15" s="5" t="inlineStr">
@@ -1657,6 +2468,24 @@
         </is>
       </c>
       <c r="J15" s="5" t="n"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="42" customHeight="1" s="12">
       <c r="A16" s="5" t="inlineStr">
@@ -1705,6 +2534,24 @@
       <c r="J16" s="5" t="inlineStr">
         <is>
           <t>Parallel stream</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>07_Databases (0.05), 13_IT_Infrastructure (0.04), 09_Expert_Systems (0.04)</t>
         </is>
       </c>
     </row>
@@ -1724,9 +2571,12 @@
       <formula>$F5="In progress"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation sqref="H5:H17" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Not started,In progress,Blocked,Ready for review,Done"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=Framework_Index!$A$2:$A$44</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2684,7 +3534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CB19"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -2713,6 +3563,26 @@
           <t>Ticketing System (Backlog)</t>
         </is>
       </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Framework_Suggested</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Framework_Confidence</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Framework_Top3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="inlineStr">
@@ -2720,8 +3590,30 @@
           <t>Use this as a lightweight Jira: each row is a ticket. Filter/sort freely.</t>
         </is>
       </c>
-    </row>
-    <row r="3"/>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers (0.10), 40_Business_Intelligence_Reconciliation (0.09), 39_Business_Intelligence_Reporting (0.09)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" s="15" t="inlineStr">
         <is>
@@ -2818,6 +3710,24 @@
           <t>Roadmap_Milestone</t>
         </is>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI (0.12), 24_Features_Public_Live_Market (0.10), 11_GUI_Pulse_Input (0.10)</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="36" customHeight="1" s="12">
       <c r="A5" s="5" t="inlineStr">
@@ -2897,6 +3807,24 @@
           <t>TRIAGE</t>
         </is>
       </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="36" customHeight="1" s="12">
       <c r="A6" s="5" t="inlineStr">
@@ -2980,6 +3908,24 @@
           <t>TRIAGE</t>
         </is>
       </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="36" customHeight="1" s="12">
       <c r="A7" s="5" t="inlineStr">
@@ -3063,6 +4009,24 @@
           <t>TRIAGE</t>
         </is>
       </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="36" customHeight="1" s="12">
       <c r="A8" s="5" t="inlineStr">
@@ -3146,6 +4110,24 @@
           <t>TRIAGE</t>
         </is>
       </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="36" customHeight="1" s="12">
       <c r="A9" s="5" t="inlineStr">
@@ -3227,6 +4209,24 @@
       <c r="S9" t="inlineStr">
         <is>
           <t>TRIAGE</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST (0.05), 07_Databases (0.04), 13_IT_Infrastructure (0.03)</t>
         </is>
       </c>
     </row>
@@ -3255,6 +4255,9 @@
         <f>IF(J10="","", "Q"&amp;ROUNDUP(MONTH(J10)/3,0)&amp;"_"&amp;TEXT(J10,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="n"/>
@@ -3281,6 +4284,9 @@
         <f>IF(J11="","", "Q"&amp;ROUNDUP(MONTH(J11)/3,0)&amp;"_"&amp;TEXT(J11,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="n"/>
@@ -3307,6 +4313,9 @@
         <f>IF(J12="","", "Q"&amp;ROUNDUP(MONTH(J12)/3,0)&amp;"_"&amp;TEXT(J12,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="n"/>
@@ -3333,6 +4342,9 @@
         <f>IF(J13="","", "Q"&amp;ROUNDUP(MONTH(J13)/3,0)&amp;"_"&amp;TEXT(J13,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="n"/>
@@ -3359,6 +4371,9 @@
         <f>IF(J14="","", "Q"&amp;ROUNDUP(MONTH(J14)/3,0)&amp;"_"&amp;TEXT(J14,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -3385,6 +4400,9 @@
         <f>IF(J15="","", "Q"&amp;ROUNDUP(MONTH(J15)/3,0)&amp;"_"&amp;TEXT(J15,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="n"/>
@@ -3411,6 +4429,9 @@
         <f>IF(J16="","", "Q"&amp;ROUNDUP(MONTH(J16)/3,0)&amp;"_"&amp;TEXT(J16,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="n"/>
@@ -3437,6 +4458,9 @@
         <f>IF(J17="","", "Q"&amp;ROUNDUP(MONTH(J17)/3,0)&amp;"_"&amp;TEXT(J17,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="n"/>
@@ -3463,6 +4487,9 @@
         <f>IF(J18="","", "Q"&amp;ROUNDUP(MONTH(J18)/3,0)&amp;"_"&amp;TEXT(J18,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="n"/>
@@ -3489,13 +4516,16 @@
         <f>IF(J19="","", "Q"&amp;ROUNDUP(MONTH(J19)/3,0)&amp;"_"&amp;TEXT(J19,"yyyy"))</f>
         <v/>
       </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation sqref="F5:F200" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"P0,P1,P2,P3"</formula1>
     </dataValidation>
@@ -3510,6 +4540,9 @@
     </dataValidation>
     <dataValidation sqref="S5:S19" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>'99_Validation'!$B$2:$B$5</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K5000 T2:T5000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=Framework_Index!$A$2:$A$44</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4235,7 +5268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4460,7 +5493,938 @@
         </is>
       </c>
     </row>
-    <row r="17"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>00_Executive_Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01_Project_Framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02_Technology_Advantage</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03_Information_Advantage</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04_Trading_Advantage</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06_Automation_Admin_AWACS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>08_Trading_Engines</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>09_Expert_Systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11_GUI_Pulse_Input</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12_Lead_and_Lag_Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13_IT_Infrastructure</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15_MLflow</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16_Modelling_Feature_Design_and_Engineering_Principles</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17_Modelling_Statistic_Cohorts</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>18_Features_Profile</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>19_Features_Performance</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21_Features_Preferences</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22_Features_Pace_Position_in_Run_PIR_RunStyle</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23_Features_Projection</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25_Ratings_Performance_POWRTG</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26_Ratings_Performance_SPDRTG</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27_Ratings_Perception_MRKRTG</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28_Ratings_Performance_TRKSPD</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29_Ratings_Performance_Grade_Benchmarks_Global_Standardization</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30_Ratings_Performance_Time_Standards</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31_Model_Simulation_Backtesting</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33_Trading_Strategies_Tote</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34_Trading_Strategies_Exchange</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35_Trading_Strategies_Fixed_Odds</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36_Trading_Strategies_Dividend_Prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>37_Trading_Strategies_cA_Continuous_Alpha</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>38_Business_Intelligence</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>39_Business_Intelligence_Reporting</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>40_Business_Intelligence_Reconciliation</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>41_Trading_Strategies_Staking_Kelly</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>42_Trading_Strategies_Staking_Isaacs</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>90_Assets_Icon_Library</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Framework_Node</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Epic_Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ticket_Count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Epic_IDs</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Ticket_IDs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>00_Executive_Summary</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01_Project_Framework</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02_Technology_Advantage</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03_Information_Advantage</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04_Trading_Advantage</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05_Glass_Cockpit_GUI</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06_Automation_Admin_AWACS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>07_Databases</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>08_Trading_Engines</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>09_Expert_Systems</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10_Pulse_Race_Status_Bet_Triggers</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11_GUI_Pulse_Input</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12_Lead_and_Lag_Analysis</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13_IT_Infrastructure</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14_ML_XGBOOST</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15_MLflow</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16_Modelling_Feature_Design_and_Engineering_Principles</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>17_Modelling_Statistic_Cohorts</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>18_Features_Profile</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>19_Features_Performance</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21_Features_Preferences</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22_Features_Pace_Position_in_Run_PIR_RunStyle</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23_Features_Projection</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24_Features_Public_Live_Market</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25_Ratings_Performance_POWRTG</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26_Ratings_Performance_SPDRTG</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27_Ratings_Perception_MRKRTG</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28_Ratings_Performance_TRKSPD</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29_Ratings_Performance_Grade_Benchmarks_Global_Standardization</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30_Ratings_Performance_Time_Standards</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31_Model_Simulation_Backtesting</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32_Trading_Strategies_Early_Mid_Late_Market</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33_Trading_Strategies_Tote</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34_Trading_Strategies_Exchange</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35_Trading_Strategies_Fixed_Odds</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36_Trading_Strategies_Dividend_Prediction</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>37_Trading_Strategies_cA_Continuous_Alpha</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>38_Business_Intelligence</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>39_Business_Intelligence_Reporting</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>40_Business_Intelligence_Reconciliation</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>41_Trading_Strategies_Staking_Kelly</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>42_Trading_Strategies_Staking_Isaacs</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>90_Assets_Icon_Library</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>